<commit_message>
[Amruta] naukari update day 4
</commit_message>
<xml_diff>
--- a/TestData/NaukariLoginDetails.xlsx
+++ b/TestData/NaukariLoginDetails.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakha\eclipse\Fresh-eclipse-workspace\Naukari\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrut\Documents\NaukariAmrutamaam\Naukari\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DC2778-0871-4EFB-9D0F-1DC23BB71E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72680E89-2496-42CE-A5F1-7C2DDFD19A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30450" yWindow="1650" windowWidth="14400" windowHeight="10545" xr2:uid="{D30C8ADD-A122-4CCD-9BF8-2CFC78D6DB52}"/>
+    <workbookView xWindow="4070" yWindow="970" windowWidth="14400" windowHeight="7270" xr2:uid="{D30C8ADD-A122-4CCD-9BF8-2CFC78D6DB52}"/>
   </bookViews>
   <sheets>
     <sheet name="naukaridata" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>8rPk_H.cZ_jmuEP</t>
+    <t>Dedicated IT professional with history of meeting company goals utilizing consistent and organized practices. Proven skills in completing black box, functional, Non-functional, Smoke, Regression, Re-testing tests, Maven, Testng, API, Selenium.</t>
   </si>
   <si>
-    <t>lakhansadewar@gmail.com</t>
+    <t>amrutamane1605@gmail.com</t>
   </si>
   <si>
-    <t>Software quality analyst with 3.2 years of experience in software quality processes, Involved in end-to-end features testing. Skills in Automation testing, Manual UI Testing, Database and API Testing.</t>
+    <t>Diliprao16</t>
   </si>
 </sst>
 </file>
@@ -69,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,28 +389,29 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="172.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>